<commit_message>
- Added 1117-Patch-20250402-02-Asset-CSC: Load list of RST Train Asset to be asociated to CSC - Added 1118-File-ExchangeRate-Daily: Load list of daily exchange rate for fx conversion - Added 1119-File-User-DisplayName: Load list of displayname to personid mapping for RFQ.PurchaseAgent - Added 1120-File-Inventory-Master: Load coswin inventory status as per data migration - Added 1211-Fix-RFQ-As-is - Added 1212-Fix-PO-As-is - Added 1214-Fix-Inventory-As-is - Added 1215-Fix-InvVendor-As-is - Added 1216-Fix-InvBalances-As-is - Added 1217-Fix-Matrectrans-As-is
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/jobplan-jobtask-pm.xlsx
+++ b/Integration Services Project2/notes/jobplan-jobtask-pm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8576A090-A403-4483-8F7C-77C8829840A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480AB421-9DD4-44D3-BA6C-892E62C25FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{42E33BE7-C02F-4CFC-BC40-A2D7D2838797}"/>
   </bookViews>
@@ -19,6 +19,9 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet5!$B$1:$E$74</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="204">
   <si>
     <t>JOBPLAN / MASTER PM?</t>
   </si>
@@ -679,6 +682,12 @@
   </si>
   <si>
     <t>WOGEN</t>
+  </si>
+  <si>
+    <t>GLCOMPONENTS</t>
+  </si>
+  <si>
+    <t>COMPVALUE</t>
   </si>
 </sst>
 </file>
@@ -789,7 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -823,12 +832,23 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2557,7 +2577,7 @@
   <dimension ref="B1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2826,20 +2846,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107E9907-C327-4F28-BAA6-B325243B6F83}">
-  <dimension ref="B1:D73"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="B1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="27.44140625" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>142</v>
       </c>
@@ -2849,8 +2871,11 @@
       <c r="D1" s="6" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>52</v>
       </c>
@@ -2860,8 +2885,11 @@
       <c r="D2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>52</v>
       </c>
@@ -2871,8 +2899,11 @@
       <c r="D3" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>52</v>
       </c>
@@ -2882,8 +2913,11 @@
       <c r="D4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>52</v>
       </c>
@@ -2893,8 +2927,11 @@
       <c r="D5" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>52</v>
       </c>
@@ -2904,8 +2941,11 @@
       <c r="D6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>52</v>
       </c>
@@ -2915,8 +2955,11 @@
       <c r="D7" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>52</v>
       </c>
@@ -2926,8 +2969,11 @@
       <c r="D8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>52</v>
       </c>
@@ -2937,8 +2983,11 @@
       <c r="D9" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>52</v>
       </c>
@@ -2948,8 +2997,11 @@
       <c r="D10" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>52</v>
       </c>
@@ -2959,8 +3011,11 @@
       <c r="D11" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>52</v>
       </c>
@@ -2970,8 +3025,11 @@
       <c r="D12" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>52</v>
       </c>
@@ -2981,8 +3039,11 @@
       <c r="D13" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>52</v>
       </c>
@@ -2992,8 +3053,11 @@
       <c r="D14" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>52</v>
       </c>
@@ -3003,8 +3067,11 @@
       <c r="D15" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>52</v>
       </c>
@@ -3014,8 +3081,11 @@
       <c r="D16" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>52</v>
       </c>
@@ -3025,8 +3095,11 @@
       <c r="D17" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>52</v>
       </c>
@@ -3036,8 +3109,11 @@
       <c r="D18" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>52</v>
       </c>
@@ -3047,8 +3123,11 @@
       <c r="D19" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>52</v>
       </c>
@@ -3058,8 +3137,11 @@
       <c r="D20" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>52</v>
       </c>
@@ -3069,8 +3151,11 @@
       <c r="D21" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>52</v>
       </c>
@@ -3080,8 +3165,11 @@
       <c r="D22" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>52</v>
       </c>
@@ -3091,8 +3179,11 @@
       <c r="D23" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>52</v>
       </c>
@@ -3102,8 +3193,11 @@
       <c r="D24" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>52</v>
       </c>
@@ -3113,8 +3207,11 @@
       <c r="D25" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>52</v>
       </c>
@@ -3124,8 +3221,11 @@
       <c r="D26" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>52</v>
       </c>
@@ -3135,8 +3235,11 @@
       <c r="D27" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>52</v>
       </c>
@@ -3146,8 +3249,11 @@
       <c r="D28" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>52</v>
       </c>
@@ -3157,8 +3263,11 @@
       <c r="D29" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>52</v>
       </c>
@@ -3168,8 +3277,11 @@
       <c r="D30" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>52</v>
       </c>
@@ -3179,8 +3291,11 @@
       <c r="D31" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>52</v>
       </c>
@@ -3190,8 +3305,11 @@
       <c r="D32" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>52</v>
       </c>
@@ -3201,8 +3319,11 @@
       <c r="D33" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E33" s="18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>52</v>
       </c>
@@ -3212,8 +3333,11 @@
       <c r="D34" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E34" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>52</v>
       </c>
@@ -3223,8 +3347,11 @@
       <c r="D35" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E35" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>52</v>
       </c>
@@ -3234,8 +3361,11 @@
       <c r="D36" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E36" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>52</v>
       </c>
@@ -3245,8 +3375,11 @@
       <c r="D37" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E37" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>52</v>
       </c>
@@ -3256,8 +3389,11 @@
       <c r="D38" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E38" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>52</v>
       </c>
@@ -3267,8 +3403,11 @@
       <c r="D39" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E39" s="18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>52</v>
       </c>
@@ -3278,8 +3417,11 @@
       <c r="D40" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E40" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>52</v>
       </c>
@@ -3289,8 +3431,11 @@
       <c r="D41" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E41" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>52</v>
       </c>
@@ -3300,8 +3445,11 @@
       <c r="D42" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E42" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>52</v>
       </c>
@@ -3311,8 +3459,11 @@
       <c r="D43" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E43" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>52</v>
       </c>
@@ -3322,8 +3473,11 @@
       <c r="D44" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E44" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>52</v>
       </c>
@@ -3333,8 +3487,11 @@
       <c r="D45" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E45" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>52</v>
       </c>
@@ -3344,8 +3501,11 @@
       <c r="D46" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E46" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>52</v>
       </c>
@@ -3355,8 +3515,11 @@
       <c r="D47" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E47" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>52</v>
       </c>
@@ -3366,8 +3529,11 @@
       <c r="D48" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E48" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>52</v>
       </c>
@@ -3377,8 +3543,11 @@
       <c r="D49" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E49" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>52</v>
       </c>
@@ -3388,8 +3557,11 @@
       <c r="D50" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E50" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>52</v>
       </c>
@@ -3399,8 +3571,11 @@
       <c r="D51" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E51" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>52</v>
       </c>
@@ -3410,8 +3585,11 @@
       <c r="D52" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E52" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>52</v>
       </c>
@@ -3421,8 +3599,11 @@
       <c r="D53" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E53" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>52</v>
       </c>
@@ -3432,8 +3613,11 @@
       <c r="D54" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E54" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>52</v>
       </c>
@@ -3443,8 +3627,11 @@
       <c r="D55" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E55" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>52</v>
       </c>
@@ -3454,8 +3641,11 @@
       <c r="D56" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E56" s="18" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>52</v>
       </c>
@@ -3465,8 +3655,11 @@
       <c r="D57" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E57" s="18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>52</v>
       </c>
@@ -3476,8 +3669,11 @@
       <c r="D58" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E58" s="18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>52</v>
       </c>
@@ -3487,8 +3683,11 @@
       <c r="D59" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E59" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>52</v>
       </c>
@@ -3498,8 +3697,11 @@
       <c r="D60" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E60" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>52</v>
       </c>
@@ -3509,8 +3711,11 @@
       <c r="D61" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E61" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>52</v>
       </c>
@@ -3520,8 +3725,11 @@
       <c r="D62" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E62" s="18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>52</v>
       </c>
@@ -3531,8 +3739,11 @@
       <c r="D63" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E63" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>52</v>
       </c>
@@ -3542,8 +3753,11 @@
       <c r="D64" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E64" s="18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>52</v>
       </c>
@@ -3553,8 +3767,11 @@
       <c r="D65" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E65" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>52</v>
       </c>
@@ -3564,8 +3781,11 @@
       <c r="D66" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E66" s="18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>52</v>
       </c>
@@ -3575,8 +3795,11 @@
       <c r="D67" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E67" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>52</v>
       </c>
@@ -3586,8 +3809,11 @@
       <c r="D68" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E68" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>52</v>
       </c>
@@ -3597,8 +3823,11 @@
       <c r="D69" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E69" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>52</v>
       </c>
@@ -3608,8 +3837,11 @@
       <c r="D70" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E70" s="18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>52</v>
       </c>
@@ -3619,8 +3851,11 @@
       <c r="D71" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E71" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>52</v>
       </c>
@@ -3630,8 +3865,11 @@
       <c r="D72" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E72" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>52</v>
       </c>
@@ -3641,8 +3879,30 @@
       <c r="D73" t="s">
         <v>168</v>
       </c>
+      <c r="E73" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>52</v>
+      </c>
+      <c r="C74" t="s">
+        <v>202</v>
+      </c>
+      <c r="D74" t="s">
+        <v>203</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>202</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:E74" xr:uid="{107E9907-C327-4F28-BAA6-B325243B6F83}">
+    <filterColumn colId="3">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Added: new Coswin's cost centre mapping - Added: migration for WOActivity - Added: as-is migration for RFQLine - Added: updated report views and stored procedures
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/jobplan-jobtask-pm.xlsx
+++ b/Integration Services Project2/notes/jobplan-jobtask-pm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480AB421-9DD4-44D3-BA6C-892E62C25FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43520952-2D24-46CF-82CD-E97BF162DC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{42E33BE7-C02F-4CFC-BC40-A2D7D2838797}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="209">
   <si>
     <t>JOBPLAN / MASTER PM?</t>
   </si>
@@ -688,6 +688,21 @@
   </si>
   <si>
     <t>COMPVALUE</t>
+  </si>
+  <si>
+    <t>FROM MRLINE</t>
+  </si>
+  <si>
+    <t>FROM INVUSELINE</t>
+  </si>
+  <si>
+    <t>MIGRATION_SOURCE=DEM-TRANSFER, FROM INVUSELINE</t>
+  </si>
+  <si>
+    <t>MIGRATION_SOURCE=RCT_ITEMS, FROM POLINE</t>
+  </si>
+  <si>
+    <t>FROM POLINE</t>
   </si>
 </sst>
 </file>
@@ -798,7 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -834,6 +849,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -2847,11 +2865,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107E9907-C327-4F28-BAA6-B325243B6F83}">
   <sheetPr filterMode="1"/>
-  <dimension ref="B1:E74"/>
+  <dimension ref="B1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2859,6 +2877,8 @@
     <col min="3" max="3" width="27.44140625" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="27.44140625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" customWidth="1"/>
+    <col min="7" max="7" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2885,7 +2905,7 @@
       <c r="D2" t="s">
         <v>168</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="16" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3085,7 +3105,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>52</v>
       </c>
@@ -3099,7 +3119,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>52</v>
       </c>
@@ -3113,7 +3133,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>52</v>
       </c>
@@ -3127,7 +3147,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="20" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>52</v>
       </c>
@@ -3141,7 +3161,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>52</v>
       </c>
@@ -3155,7 +3175,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>52</v>
       </c>
@@ -3169,7 +3189,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>52</v>
       </c>
@@ -3179,11 +3199,11 @@
       <c r="D23" t="s">
         <v>168</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="16" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>52</v>
       </c>
@@ -3193,11 +3213,11 @@
       <c r="D24" t="s">
         <v>168</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="16" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>52</v>
       </c>
@@ -3211,7 +3231,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>52</v>
       </c>
@@ -3225,7 +3245,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>52</v>
       </c>
@@ -3235,11 +3255,14 @@
       <c r="D27" t="s">
         <v>168</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>52</v>
       </c>
@@ -3249,11 +3272,11 @@
       <c r="D28" t="s">
         <v>169</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="16" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>52</v>
       </c>
@@ -3263,11 +3286,14 @@
       <c r="D29" t="s">
         <v>169</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="16" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>52</v>
       </c>
@@ -3281,7 +3307,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>52</v>
       </c>
@@ -3295,7 +3321,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>52</v>
       </c>
@@ -3309,7 +3335,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>52</v>
       </c>
@@ -3323,7 +3349,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>52</v>
       </c>
@@ -3333,11 +3359,17 @@
       <c r="D34" t="s">
         <v>169</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="16" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F34" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>52</v>
       </c>
@@ -3347,11 +3379,14 @@
       <c r="D35" t="s">
         <v>169</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>52</v>
       </c>
@@ -3361,11 +3396,11 @@
       <c r="D36" t="s">
         <v>169</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>52</v>
       </c>
@@ -3375,11 +3410,11 @@
       <c r="D37" t="s">
         <v>169</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="16" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>52</v>
       </c>
@@ -3389,11 +3424,11 @@
       <c r="D38" t="s">
         <v>169</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>52</v>
       </c>
@@ -3407,7 +3442,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="40" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>52</v>
       </c>
@@ -3421,7 +3456,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>52</v>
       </c>
@@ -3435,7 +3470,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>52</v>
       </c>
@@ -3449,7 +3484,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>52</v>
       </c>
@@ -3463,7 +3498,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>52</v>
       </c>
@@ -3477,7 +3512,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>52</v>
       </c>
@@ -3491,7 +3526,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>52</v>
       </c>
@@ -3501,11 +3536,11 @@
       <c r="D46" t="s">
         <v>169</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E46" s="16" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>52</v>
       </c>
@@ -3515,11 +3550,11 @@
       <c r="D47" t="s">
         <v>169</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>52</v>
       </c>
@@ -3529,11 +3564,11 @@
       <c r="D48" t="s">
         <v>169</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="16" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>52</v>
       </c>
@@ -3543,11 +3578,11 @@
       <c r="D49" t="s">
         <v>169</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="16" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>52</v>
       </c>
@@ -3561,7 +3596,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="51" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>52</v>
       </c>
@@ -3575,7 +3610,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>52</v>
       </c>
@@ -3589,7 +3624,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>52</v>
       </c>
@@ -3599,11 +3634,11 @@
       <c r="D53" t="s">
         <v>169</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>52</v>
       </c>
@@ -3617,7 +3652,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="55" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>52</v>
       </c>
@@ -3631,7 +3666,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="56" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>52</v>
       </c>
@@ -3645,7 +3680,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="57" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>52</v>
       </c>
@@ -3659,7 +3694,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="58" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>52</v>
       </c>
@@ -3673,7 +3708,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>52</v>
       </c>
@@ -3683,11 +3718,14 @@
       <c r="D59" t="s">
         <v>169</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="E59" s="16" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F59" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>52</v>
       </c>
@@ -3697,11 +3735,14 @@
       <c r="D60" t="s">
         <v>168</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E60" s="16" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>52</v>
       </c>
@@ -3711,11 +3752,11 @@
       <c r="D61" t="s">
         <v>169</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="E61" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="62" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>52</v>
       </c>
@@ -3729,7 +3770,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>52</v>
       </c>
@@ -3739,11 +3780,11 @@
       <c r="D63" t="s">
         <v>168</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E63" s="16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>52</v>
       </c>
@@ -3757,7 +3798,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="65" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>52</v>
       </c>
@@ -3771,7 +3812,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>52</v>
       </c>
@@ -3785,7 +3826,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>52</v>
       </c>
@@ -3795,11 +3836,14 @@
       <c r="D67" t="s">
         <v>168</v>
       </c>
-      <c r="E67" s="7" t="s">
+      <c r="E67" s="16" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F67" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>52</v>
       </c>
@@ -3809,11 +3853,14 @@
       <c r="D68" t="s">
         <v>168</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E68" s="9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="69" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F68" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>52</v>
       </c>
@@ -3827,7 +3874,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>52</v>
       </c>
@@ -3841,7 +3888,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="71" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>52</v>
       </c>
@@ -3855,7 +3902,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>52</v>
       </c>
@@ -3865,11 +3912,11 @@
       <c r="D72" t="s">
         <v>168</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="E72" s="16" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>52</v>
       </c>
@@ -3879,11 +3926,11 @@
       <c r="D73" t="s">
         <v>168</v>
       </c>
-      <c r="E73" s="7" t="s">
+      <c r="E73" s="16" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>52</v>
       </c>
@@ -3893,7 +3940,7 @@
       <c r="D74" t="s">
         <v>203</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="E74" s="16" t="s">
         <v>202</v>
       </c>
     </row>

</xml_diff>